<commit_message>
Rigorous Invigilation Successfully Done
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="144">
   <si>
     <t xml:space="preserve"> 08:30 - 10:30 </t>
   </si>
@@ -345,6 +345,16 @@
     <t>Information Theory and Coding</t>
   </si>
   <si>
+    <t>CS302</t>
+  </si>
+  <si>
+    <t>Modeling and Simulation</t>
+  </si>
+  <si>
+    <t>55
+[R]</t>
+  </si>
+  <si>
     <t>SC431</t>
   </si>
   <si>
@@ -355,16 +365,6 @@
 [L]</t>
   </si>
   <si>
-    <t>CS302</t>
-  </si>
-  <si>
-    <t>Modeling and Simulation</t>
-  </si>
-  <si>
-    <t>55
-[R]</t>
-  </si>
-  <si>
     <t>IT415</t>
   </si>
   <si>
@@ -381,6 +381,14 @@
     <t>Computer Networks</t>
   </si>
   <si>
+    <t>57
+[L]</t>
+  </si>
+  <si>
+    <t>52
+[L]</t>
+  </si>
+  <si>
     <t>EL520</t>
   </si>
   <si>
@@ -413,14 +421,26 @@
     <t>Models of Computation</t>
   </si>
   <si>
-    <t>38
+    <t>78
 [R]</t>
   </si>
   <si>
+    <t>58
+[R]</t>
+  </si>
+  <si>
     <t>IT325</t>
   </si>
   <si>
     <t>Introduction to Cryptology</t>
+  </si>
+  <si>
+    <t>94
+[L]</t>
+  </si>
+  <si>
+    <t>18
+[L]</t>
   </si>
   <si>
     <t>IT468</t>
@@ -439,18 +459,14 @@
     <t>Systems Approach to Sustainable Development</t>
   </si>
   <si>
-    <t>4
+    <t>CT516</t>
+  </si>
+  <si>
+    <t>Advanced Digital Communications</t>
+  </si>
+  <si>
+    <t>7
 [R]</t>
-  </si>
-  <si>
-    <t>CT516</t>
-  </si>
-  <si>
-    <t>Advanced Digital Communications</t>
-  </si>
-  <si>
-    <t>7
-[L]</t>
   </si>
   <si>
     <t>EL516</t>
@@ -2952,7 +2968,7 @@
       <c r="AF35" t="s" s="3">
         <v>101</v>
       </c>
-      <c r="AJ35" t="s" s="3">
+      <c r="AI35" t="s" s="3">
         <v>102</v>
       </c>
       <c r="AL35" s="38"/>
@@ -3004,10 +3020,10 @@
         <v>6</v>
       </c>
       <c r="AI37" t="s" s="3">
+        <v>108</v>
+      </c>
+      <c r="AJ37" t="s" s="3">
         <v>7</v>
-      </c>
-      <c r="AJ37" t="s" s="3">
-        <v>108</v>
       </c>
       <c r="AL37" s="38"/>
     </row>
@@ -3040,10 +3056,10 @@
         <v>110</v>
       </c>
       <c r="AH38" t="s" s="5">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="AI38" t="s" s="5">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="AL38" s="38"/>
     </row>
@@ -3066,12 +3082,12 @@
       <c r="V39" s="27"/>
       <c r="AC39" s="38"/>
       <c r="AE39" t="s" s="50">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="AF39" t="s" s="9">
-        <v>112</v>
-      </c>
-      <c r="AI39" t="s" s="9">
+        <v>114</v>
+      </c>
+      <c r="AH39" t="s" s="9">
         <v>37</v>
       </c>
       <c r="AL39" s="38"/>
@@ -3110,16 +3126,16 @@
       <c r="AB40" s="41"/>
       <c r="AC40" s="43"/>
       <c r="AE40" t="s" s="89">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AF40" t="s" s="90">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AG40" s="41"/>
-      <c r="AH40" s="41"/>
-      <c r="AI40" t="s" s="90">
-        <v>115</v>
-      </c>
+      <c r="AH40" t="s" s="90">
+        <v>117</v>
+      </c>
+      <c r="AI40" s="41"/>
       <c r="AJ40" s="41"/>
       <c r="AK40" s="41"/>
       <c r="AL40" s="43"/>
@@ -3254,13 +3270,13 @@
       <c r="D44" s="27"/>
       <c r="K44" s="38"/>
       <c r="M44" t="s" s="31">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="R44" t="s" s="2">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="T44" s="38"/>
       <c r="V44" s="27"/>
@@ -3276,25 +3292,25 @@
       <c r="D45" s="27"/>
       <c r="K45" s="38"/>
       <c r="M45" t="s" s="33">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="N45" t="s" s="3">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="P45" t="s" s="3">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="Q45" t="s" s="3">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="T45" s="38"/>
       <c r="V45" s="27"/>
       <c r="AC45" s="38"/>
       <c r="AE45" t="s" s="33">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AF45" t="s" s="3">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="AH45" t="s" s="3">
         <v>6</v>
@@ -3306,7 +3322,7 @@
         <v>8</v>
       </c>
       <c r="AK45" t="s" s="3">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="AL45" s="38"/>
     </row>
@@ -3316,16 +3332,16 @@
       <c r="D46" s="27"/>
       <c r="K46" s="38"/>
       <c r="M46" t="s" s="33">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="N46" t="s" s="3">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="P46" t="s" s="3">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="Q46" t="s" s="3">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="T46" s="38"/>
       <c r="V46" s="27"/>
@@ -3339,13 +3355,13 @@
       <c r="D47" s="27"/>
       <c r="K47" s="38"/>
       <c r="M47" t="s" s="33">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="N47" t="s" s="3">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="Q47" t="s" s="3">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="T47" s="38"/>
       <c r="V47" s="27"/>
@@ -3365,10 +3381,10 @@
       <c r="V48" s="27"/>
       <c r="AC48" s="38"/>
       <c r="AE48" t="s" s="49">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AF48" t="s" s="5">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="AH48" t="s" s="5">
         <v>30</v>
@@ -3386,13 +3402,13 @@
       <c r="D49" s="27"/>
       <c r="K49" s="38"/>
       <c r="M49" t="s" s="84">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="N49" t="s" s="7">
-        <v>128</v>
-      </c>
-      <c r="Q49" t="s" s="7">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="P49" t="s" s="7">
+        <v>63</v>
       </c>
       <c r="T49" s="38"/>
       <c r="V49" s="27"/>
@@ -3408,13 +3424,13 @@
       <c r="D50" s="27"/>
       <c r="K50" s="38"/>
       <c r="M50" t="s" s="50">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N50" t="s" s="9">
-        <v>131</v>
-      </c>
-      <c r="Q50" t="s" s="9">
-        <v>132</v>
+        <v>135</v>
+      </c>
+      <c r="P50" t="s" s="9">
+        <v>136</v>
       </c>
       <c r="T50" s="38"/>
       <c r="V50" s="27"/>
@@ -3434,16 +3450,16 @@
       <c r="J51" s="41"/>
       <c r="K51" s="43"/>
       <c r="M51" t="s" s="89">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="N51" t="s" s="90">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="O51" s="41"/>
-      <c r="P51" s="41"/>
-      <c r="Q51" t="s" s="90">
+      <c r="P51" t="s" s="90">
         <v>52</v>
       </c>
+      <c r="Q51" s="41"/>
       <c r="R51" s="41"/>
       <c r="S51" s="41"/>
       <c r="T51" s="43"/>

</xml_diff>

<commit_message>
Reading from Excel done
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -120,6 +120,16 @@
 [L]</t>
   </si>
   <si>
+    <t>IT543</t>
+  </si>
+  <si>
+    <t>Adv. Logic for Computer Science</t>
+  </si>
+  <si>
+    <t>15
+[L]</t>
+  </si>
+  <si>
     <t>CT513</t>
   </si>
   <si>
@@ -130,16 +140,6 @@
 [L]</t>
   </si>
   <si>
-    <t>IT543</t>
-  </si>
-  <si>
-    <t>Adv. Logic for Computer Science</t>
-  </si>
-  <si>
-    <t>15
-[L]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 14:00 - 16:00 </t>
   </si>
   <si>
@@ -329,6 +329,12 @@
 [L]</t>
   </si>
   <si>
+    <t>CT512</t>
+  </si>
+  <si>
+    <t>Information Theory and Coding</t>
+  </si>
+  <si>
     <t>IT410</t>
   </si>
   <si>
@@ -339,10 +345,14 @@
 [R]</t>
   </si>
   <si>
-    <t>CT512</t>
-  </si>
-  <si>
-    <t>Information Theory and Coding</t>
+    <t>IT415</t>
+  </si>
+  <si>
+    <t>Software Testing and Quality Analysis</t>
+  </si>
+  <si>
+    <t>5
+[R]</t>
   </si>
   <si>
     <t>CS302</t>
@@ -365,16 +375,6 @@
 [L]</t>
   </si>
   <si>
-    <t>IT415</t>
-  </si>
-  <si>
-    <t>Software Testing and Quality Analysis</t>
-  </si>
-  <si>
-    <t>5
-[R]</t>
-  </si>
-  <si>
     <t>IT694</t>
   </si>
   <si>
@@ -389,12 +389,6 @@
 [L]</t>
   </si>
   <si>
-    <t>EL520</t>
-  </si>
-  <si>
-    <t>Digital System Design using Verilog</t>
-  </si>
-  <si>
     <t>SC522</t>
   </si>
   <si>
@@ -403,6 +397,12 @@
   <si>
     <t>26
 [L]</t>
+  </si>
+  <si>
+    <t>EL520</t>
+  </si>
+  <si>
+    <t>Digital System Design using Verilog</t>
   </si>
   <si>
     <t>CS201</t>
@@ -1531,7 +1531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="true"/>
@@ -1868,6 +1868,10 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="40" borderId="22" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="centerContinuous" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true">
@@ -2329,9 +2333,10 @@
       <c r="N18" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="T18" t="s" s="52">
+      <c r="S18" t="s" s="9">
         <v>34</v>
       </c>
+      <c r="T18" s="38"/>
       <c r="V18" s="27"/>
       <c r="AC18" s="38"/>
       <c r="AE18" t="s" s="50">
@@ -2356,10 +2361,9 @@
       <c r="N19" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="S19" t="s" s="9">
+      <c r="T19" t="s" s="52">
         <v>37</v>
       </c>
-      <c r="T19" s="38"/>
       <c r="V19" s="27"/>
       <c r="AC19" s="38"/>
       <c r="AE19" s="27"/>
@@ -2817,24 +2821,24 @@
       <c r="R32" s="26"/>
       <c r="S32" s="26"/>
       <c r="T32" s="36"/>
-      <c r="V32" t="s" s="114">
+      <c r="V32" t="s" s="115">
         <v>38</v>
       </c>
       <c r="W32" s="26"/>
       <c r="X32" s="26"/>
-      <c r="Y32" t="s" s="115">
+      <c r="Y32" t="s" s="116">
         <v>1</v>
       </c>
       <c r="Z32" s="26"/>
       <c r="AA32" s="26"/>
       <c r="AB32" s="26"/>
       <c r="AC32" s="36"/>
-      <c r="AE32" t="s" s="119">
+      <c r="AE32" t="s" s="120">
         <v>39</v>
       </c>
       <c r="AF32" s="26"/>
       <c r="AG32" s="26"/>
-      <c r="AH32" t="s" s="118">
+      <c r="AH32" t="s" s="119">
         <v>1</v>
       </c>
       <c r="AI32" s="26"/>
@@ -2968,8 +2972,14 @@
       <c r="AF35" t="s" s="3">
         <v>101</v>
       </c>
+      <c r="AH35" t="s" s="3">
+        <v>6</v>
+      </c>
       <c r="AI35" t="s" s="3">
         <v>102</v>
+      </c>
+      <c r="AJ35" t="s" s="3">
+        <v>7</v>
       </c>
       <c r="AL35" s="38"/>
     </row>
@@ -2996,7 +3006,7 @@
       <c r="AF36" t="s" s="3">
         <v>104</v>
       </c>
-      <c r="AJ36" t="s" s="3">
+      <c r="AI36" t="s" s="3">
         <v>105</v>
       </c>
       <c r="AL36" s="38"/>
@@ -3016,14 +3026,8 @@
       <c r="AF37" t="s" s="3">
         <v>107</v>
       </c>
-      <c r="AH37" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="AI37" t="s" s="3">
+      <c r="AJ37" t="s" s="3">
         <v>108</v>
-      </c>
-      <c r="AJ37" t="s" s="3">
-        <v>7</v>
       </c>
       <c r="AL37" s="38"/>
     </row>
@@ -3076,9 +3080,10 @@
       <c r="N39" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="T39" t="s" s="52">
-        <v>97</v>
-      </c>
+      <c r="S39" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="T39" s="38"/>
       <c r="V39" s="27"/>
       <c r="AC39" s="38"/>
       <c r="AE39" t="s" s="50">
@@ -3088,7 +3093,7 @@
         <v>114</v>
       </c>
       <c r="AH39" t="s" s="9">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="AL39" s="38"/>
     </row>
@@ -3104,19 +3109,19 @@
       <c r="J40" s="41"/>
       <c r="K40" s="43"/>
       <c r="M40" t="s" s="89">
+        <v>97</v>
+      </c>
+      <c r="N40" t="s" s="90">
         <v>98</v>
-      </c>
-      <c r="N40" t="s" s="90">
-        <v>99</v>
       </c>
       <c r="O40" s="41"/>
       <c r="P40" s="41"/>
       <c r="Q40" s="41"/>
       <c r="R40" s="41"/>
-      <c r="S40" t="s" s="90">
-        <v>49</v>
-      </c>
-      <c r="T40" s="43"/>
+      <c r="S40" s="41"/>
+      <c r="T40" t="s" s="112">
+        <v>99</v>
+      </c>
       <c r="V40" s="40"/>
       <c r="W40" s="41"/>
       <c r="X40" s="41"/>
@@ -3126,14 +3131,14 @@
       <c r="AB40" s="41"/>
       <c r="AC40" s="43"/>
       <c r="AE40" t="s" s="89">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF40" t="s" s="90">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AG40" s="41"/>
       <c r="AH40" t="s" s="90">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="AI40" s="41"/>
       <c r="AJ40" s="41"/>
@@ -3145,48 +3150,48 @@
         <v>17</v>
       </c>
       <c r="C42" s="24"/>
-      <c r="D42" t="s" s="128">
+      <c r="D42" t="s" s="129">
         <v>0</v>
       </c>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
-      <c r="G42" t="s" s="131">
+      <c r="G42" t="s" s="132">
         <v>1</v>
       </c>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
       <c r="K42" s="36"/>
-      <c r="M42" t="s" s="137">
+      <c r="M42" t="s" s="138">
         <v>18</v>
       </c>
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
-      <c r="P42" t="s" s="138">
+      <c r="P42" t="s" s="139">
         <v>1</v>
       </c>
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
       <c r="S42" s="26"/>
       <c r="T42" s="36"/>
-      <c r="V42" t="s" s="142">
+      <c r="V42" t="s" s="143">
         <v>38</v>
       </c>
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
-      <c r="Y42" t="s" s="141">
+      <c r="Y42" t="s" s="142">
         <v>1</v>
       </c>
       <c r="Z42" s="26"/>
       <c r="AA42" s="26"/>
       <c r="AB42" s="26"/>
       <c r="AC42" s="36"/>
-      <c r="AE42" t="s" s="145">
+      <c r="AE42" t="s" s="146">
         <v>39</v>
       </c>
       <c r="AF42" s="26"/>
       <c r="AG42" s="26"/>
-      <c r="AH42" t="s" s="146">
+      <c r="AH42" t="s" s="147">
         <v>1</v>
       </c>
       <c r="AI42" s="26"/>
@@ -3264,7 +3269,7 @@
     </row>
     <row r="44">
       <c r="B44" s="23"/>
-      <c r="C44" t="s" s="129">
+      <c r="C44" t="s" s="130">
         <v>3</v>
       </c>
       <c r="D44" s="27"/>
@@ -3286,7 +3291,7 @@
     </row>
     <row r="45">
       <c r="B45" s="23"/>
-      <c r="C45" t="s" s="130">
+      <c r="C45" t="s" s="131">
         <v>10</v>
       </c>
       <c r="D45" s="27"/>
@@ -3371,7 +3376,7 @@
     </row>
     <row r="48">
       <c r="B48" s="23"/>
-      <c r="C48" t="s" s="132">
+      <c r="C48" t="s" s="133">
         <v>14</v>
       </c>
       <c r="D48" s="27"/>
@@ -3396,7 +3401,7 @@
     </row>
     <row r="49">
       <c r="B49" s="23"/>
-      <c r="C49" t="s" s="133">
+      <c r="C49" t="s" s="134">
         <v>53</v>
       </c>
       <c r="D49" s="27"/>
@@ -3418,7 +3423,7 @@
     </row>
     <row r="50">
       <c r="B50" s="23"/>
-      <c r="C50" t="s" s="134">
+      <c r="C50" t="s" s="135">
         <v>15</v>
       </c>
       <c r="D50" s="27"/>

</xml_diff>